<commit_message>
added async db integeration
</commit_message>
<xml_diff>
--- a/app/website_monitor/domainler.xlsx
+++ b/app/website_monitor/domainler.xlsx
@@ -655,10 +655,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S2" t="n">
+        <v>34096</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
@@ -685,15 +683,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y2" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
@@ -782,10 +776,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>35210</t>
-        </is>
+      <c r="S3" t="n">
+        <v>35210</v>
       </c>
       <c r="T3" t="inlineStr">
         <is>
@@ -812,15 +804,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>38.4127</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>27.1384</t>
-        </is>
+      <c r="Y3" t="n">
+        <v>38.4127</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>27.1384</v>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
@@ -909,10 +897,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S4" t="n">
+        <v>16250</v>
       </c>
       <c r="T4" t="inlineStr">
         <is>
@@ -939,15 +925,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y4" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA4" t="inlineStr">
         <is>
@@ -1036,10 +1018,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S5" t="n">
+        <v>16250</v>
       </c>
       <c r="T5" t="inlineStr">
         <is>
@@ -1066,15 +1046,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z5" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y5" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA5" t="inlineStr">
         <is>
@@ -1163,10 +1139,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S6" t="n">
+        <v>34096</v>
       </c>
       <c r="T6" t="inlineStr">
         <is>
@@ -1193,15 +1167,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z6" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y6" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA6" t="inlineStr">
         <is>
@@ -1290,10 +1260,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>35210</t>
-        </is>
+      <c r="S7" t="n">
+        <v>35210</v>
       </c>
       <c r="T7" t="inlineStr">
         <is>
@@ -1320,15 +1288,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>38.4127</t>
-        </is>
-      </c>
-      <c r="Z7" t="inlineStr">
-        <is>
-          <t>27.1384</t>
-        </is>
+      <c r="Y7" t="n">
+        <v>38.4127</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>27.1384</v>
       </c>
       <c r="AA7" t="inlineStr">
         <is>
@@ -1417,10 +1381,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S8" t="n">
+        <v>34096</v>
       </c>
       <c r="T8" t="inlineStr">
         <is>
@@ -1447,15 +1409,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y8" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z8" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y8" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA8" t="inlineStr">
         <is>
@@ -1544,10 +1502,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S9" t="n">
+        <v>34096</v>
       </c>
       <c r="T9" t="inlineStr">
         <is>
@@ -1574,15 +1530,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y9" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z9" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y9" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA9" t="inlineStr">
         <is>
@@ -1671,10 +1623,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S10" t="n">
+        <v>34096</v>
       </c>
       <c r="T10" t="inlineStr">
         <is>
@@ -1701,15 +1651,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y10" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z10" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y10" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA10" t="inlineStr">
         <is>
@@ -1798,10 +1744,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S11" t="n">
+        <v>34096</v>
       </c>
       <c r="T11" t="inlineStr">
         <is>
@@ -1828,15 +1772,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y11" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z11" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y11" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA11" t="inlineStr">
         <is>
@@ -1925,10 +1865,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S12" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S12" t="n">
+        <v>34096</v>
       </c>
       <c r="T12" t="inlineStr">
         <is>
@@ -1955,15 +1893,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y12" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z12" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y12" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA12" t="inlineStr">
         <is>
@@ -2052,10 +1986,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S13" t="n">
+        <v>34096</v>
       </c>
       <c r="T13" t="inlineStr">
         <is>
@@ -2082,15 +2014,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y13" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z13" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y13" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA13" t="inlineStr">
         <is>
@@ -2179,10 +2107,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>35210</t>
-        </is>
+      <c r="S14" t="n">
+        <v>35210</v>
       </c>
       <c r="T14" t="inlineStr">
         <is>
@@ -2209,15 +2135,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y14" t="inlineStr">
-        <is>
-          <t>38.4127</t>
-        </is>
-      </c>
-      <c r="Z14" t="inlineStr">
-        <is>
-          <t>27.1384</t>
-        </is>
+      <c r="Y14" t="n">
+        <v>38.4127</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>27.1384</v>
       </c>
       <c r="AA14" t="inlineStr">
         <is>
@@ -2306,10 +2228,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>35210</t>
-        </is>
+      <c r="S15" t="n">
+        <v>35210</v>
       </c>
       <c r="T15" t="inlineStr">
         <is>
@@ -2336,15 +2256,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y15" t="inlineStr">
-        <is>
-          <t>38.4127</t>
-        </is>
-      </c>
-      <c r="Z15" t="inlineStr">
-        <is>
-          <t>27.1384</t>
-        </is>
+      <c r="Y15" t="n">
+        <v>38.4127</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>27.1384</v>
       </c>
       <c r="AA15" t="inlineStr">
         <is>
@@ -2433,10 +2349,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S16" t="n">
+        <v>16250</v>
       </c>
       <c r="T16" t="inlineStr">
         <is>
@@ -2463,15 +2377,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y16" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z16" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y16" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA16" t="inlineStr">
         <is>
@@ -2560,10 +2470,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S17" t="n">
+        <v>16250</v>
       </c>
       <c r="T17" t="inlineStr">
         <is>
@@ -2590,15 +2498,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y17" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z17" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y17" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA17" t="inlineStr">
         <is>
@@ -2687,10 +2591,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S18" t="n">
+        <v>16250</v>
       </c>
       <c r="T18" t="inlineStr">
         <is>
@@ -2717,15 +2619,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y18" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z18" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y18" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA18" t="inlineStr">
         <is>
@@ -2814,10 +2712,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S19" t="n">
+        <v>16250</v>
       </c>
       <c r="T19" t="inlineStr">
         <is>
@@ -2844,15 +2740,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y19" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z19" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y19" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA19" t="inlineStr">
         <is>
@@ -2941,10 +2833,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S20" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S20" t="n">
+        <v>16250</v>
       </c>
       <c r="T20" t="inlineStr">
         <is>
@@ -2971,15 +2861,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y20" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z20" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y20" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA20" t="inlineStr">
         <is>
@@ -3068,10 +2954,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S21" t="n">
+        <v>16250</v>
       </c>
       <c r="T21" t="inlineStr">
         <is>
@@ -3098,15 +2982,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y21" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z21" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y21" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA21" t="inlineStr">
         <is>
@@ -3195,10 +3075,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S22" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S22" t="n">
+        <v>16250</v>
       </c>
       <c r="T22" t="inlineStr">
         <is>
@@ -3225,15 +3103,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y22" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z22" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y22" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA22" t="inlineStr">
         <is>
@@ -3322,10 +3196,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S23" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S23" t="n">
+        <v>16250</v>
       </c>
       <c r="T23" t="inlineStr">
         <is>
@@ -3352,15 +3224,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y23" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z23" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y23" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA23" t="inlineStr">
         <is>
@@ -3449,10 +3317,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S24" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S24" t="n">
+        <v>34096</v>
       </c>
       <c r="T24" t="inlineStr">
         <is>
@@ -3479,15 +3345,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y24" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z24" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y24" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA24" t="inlineStr">
         <is>
@@ -3576,10 +3438,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S25" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S25" t="n">
+        <v>34096</v>
       </c>
       <c r="T25" t="inlineStr">
         <is>
@@ -3606,15 +3466,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y25" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z25" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y25" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA25" t="inlineStr">
         <is>
@@ -3703,10 +3559,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S26" t="inlineStr">
-        <is>
-          <t>35210</t>
-        </is>
+      <c r="S26" t="n">
+        <v>35210</v>
       </c>
       <c r="T26" t="inlineStr">
         <is>
@@ -3733,15 +3587,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y26" t="inlineStr">
-        <is>
-          <t>38.4127</t>
-        </is>
-      </c>
-      <c r="Z26" t="inlineStr">
-        <is>
-          <t>27.1384</t>
-        </is>
+      <c r="Y26" t="n">
+        <v>38.4127</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>27.1384</v>
       </c>
       <c r="AA26" t="inlineStr">
         <is>
@@ -3830,10 +3680,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S27" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S27" t="n">
+        <v>34096</v>
       </c>
       <c r="T27" t="inlineStr">
         <is>
@@ -3860,15 +3708,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y27" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z27" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y27" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA27" t="inlineStr">
         <is>
@@ -3957,10 +3801,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S28" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S28" t="n">
+        <v>34096</v>
       </c>
       <c r="T28" t="inlineStr">
         <is>
@@ -3987,15 +3829,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y28" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z28" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y28" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA28" t="inlineStr">
         <is>
@@ -4084,10 +3922,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S29" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S29" t="n">
+        <v>34096</v>
       </c>
       <c r="T29" t="inlineStr">
         <is>
@@ -4114,15 +3950,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y29" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z29" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y29" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA29" t="inlineStr">
         <is>
@@ -4211,10 +4043,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S30" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S30" t="n">
+        <v>34096</v>
       </c>
       <c r="T30" t="inlineStr">
         <is>
@@ -4241,15 +4071,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y30" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z30" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y30" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA30" t="inlineStr">
         <is>
@@ -4338,10 +4164,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S31" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S31" t="n">
+        <v>16250</v>
       </c>
       <c r="T31" t="inlineStr">
         <is>
@@ -4368,15 +4192,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y31" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z31" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y31" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA31" t="inlineStr">
         <is>
@@ -4465,10 +4285,8 @@
           <t>AS47583 Hostinger International Limited</t>
         </is>
       </c>
-      <c r="S32" t="inlineStr">
-        <is>
-          <t>7941</t>
-        </is>
+      <c r="S32" t="n">
+        <v>7941</v>
       </c>
       <c r="T32" t="inlineStr">
         <is>
@@ -4495,15 +4313,11 @@
           <t>EU</t>
         </is>
       </c>
-      <c r="Y32" t="inlineStr">
-        <is>
-          <t>52.6958</t>
-        </is>
-      </c>
-      <c r="Z32" t="inlineStr">
-        <is>
-          <t>6.1944</t>
-        </is>
+      <c r="Y32" t="n">
+        <v>52.6958</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>6.1944</v>
       </c>
       <c r="AA32" t="inlineStr">
         <is>
@@ -4592,10 +4406,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S33" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S33" t="n">
+        <v>34096</v>
       </c>
       <c r="T33" t="inlineStr">
         <is>
@@ -4622,15 +4434,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y33" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z33" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y33" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA33" t="inlineStr">
         <is>
@@ -4719,10 +4527,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S34" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S34" t="n">
+        <v>16250</v>
       </c>
       <c r="T34" t="inlineStr">
         <is>
@@ -4749,15 +4555,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y34" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z34" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y34" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA34" t="inlineStr">
         <is>
@@ -4846,10 +4648,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S35" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S35" t="n">
+        <v>16250</v>
       </c>
       <c r="T35" t="inlineStr">
         <is>
@@ -4876,15 +4676,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y35" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z35" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y35" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA35" t="inlineStr">
         <is>
@@ -4973,10 +4769,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S36" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S36" t="n">
+        <v>34096</v>
       </c>
       <c r="T36" t="inlineStr">
         <is>
@@ -5003,15 +4797,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y36" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z36" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y36" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z36" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA36" t="inlineStr">
         <is>
@@ -5100,10 +4890,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S37" t="inlineStr">
-        <is>
-          <t>35210</t>
-        </is>
+      <c r="S37" t="n">
+        <v>35210</v>
       </c>
       <c r="T37" t="inlineStr">
         <is>
@@ -5130,15 +4918,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y37" t="inlineStr">
-        <is>
-          <t>38.4127</t>
-        </is>
-      </c>
-      <c r="Z37" t="inlineStr">
-        <is>
-          <t>27.1384</t>
-        </is>
+      <c r="Y37" t="n">
+        <v>38.4127</v>
+      </c>
+      <c r="Z37" t="n">
+        <v>27.1384</v>
       </c>
       <c r="AA37" t="inlineStr">
         <is>
@@ -5227,10 +5011,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S38" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S38" t="n">
+        <v>34096</v>
       </c>
       <c r="T38" t="inlineStr">
         <is>
@@ -5257,15 +5039,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y38" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z38" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y38" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z38" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA38" t="inlineStr">
         <is>
@@ -5354,10 +5132,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S39" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S39" t="n">
+        <v>16250</v>
       </c>
       <c r="T39" t="inlineStr">
         <is>
@@ -5384,15 +5160,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y39" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z39" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y39" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z39" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA39" t="inlineStr">
         <is>
@@ -5481,10 +5253,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S40" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S40" t="n">
+        <v>34096</v>
       </c>
       <c r="T40" t="inlineStr">
         <is>
@@ -5511,15 +5281,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y40" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z40" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y40" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z40" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA40" t="inlineStr">
         <is>
@@ -5608,10 +5374,8 @@
           <t>AS16276 OVH SAS</t>
         </is>
       </c>
-      <c r="S41" t="inlineStr">
-        <is>
-          <t>60306</t>
-        </is>
+      <c r="S41" t="n">
+        <v>60306</v>
       </c>
       <c r="T41" t="inlineStr">
         <is>
@@ -5638,15 +5402,11 @@
           <t>EU</t>
         </is>
       </c>
-      <c r="Y41" t="inlineStr">
-        <is>
-          <t>50.1155</t>
-        </is>
-      </c>
-      <c r="Z41" t="inlineStr">
-        <is>
-          <t>8.6842</t>
-        </is>
+      <c r="Y41" t="n">
+        <v>50.1155</v>
+      </c>
+      <c r="Z41" t="n">
+        <v>8.684200000000001</v>
       </c>
       <c r="AA41" t="inlineStr">
         <is>
@@ -5735,10 +5495,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S42" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S42" t="n">
+        <v>34096</v>
       </c>
       <c r="T42" t="inlineStr">
         <is>
@@ -5765,15 +5523,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y42" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z42" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y42" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z42" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA42" t="inlineStr">
         <is>
@@ -5862,10 +5616,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S43" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S43" t="n">
+        <v>34096</v>
       </c>
       <c r="T43" t="inlineStr">
         <is>
@@ -5892,15 +5644,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y43" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z43" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y43" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z43" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA43" t="inlineStr">
         <is>
@@ -5989,10 +5737,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S44" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S44" t="n">
+        <v>34096</v>
       </c>
       <c r="T44" t="inlineStr">
         <is>
@@ -6019,15 +5765,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y44" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z44" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y44" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z44" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA44" t="inlineStr">
         <is>
@@ -6116,10 +5858,8 @@
           <t>AS16276 OVH SAS</t>
         </is>
       </c>
-      <c r="S45" t="inlineStr">
-        <is>
-          <t>60306</t>
-        </is>
+      <c r="S45" t="n">
+        <v>60306</v>
       </c>
       <c r="T45" t="inlineStr">
         <is>
@@ -6146,15 +5886,11 @@
           <t>EU</t>
         </is>
       </c>
-      <c r="Y45" t="inlineStr">
-        <is>
-          <t>50.1155</t>
-        </is>
-      </c>
-      <c r="Z45" t="inlineStr">
-        <is>
-          <t>8.6842</t>
-        </is>
+      <c r="Y45" t="n">
+        <v>50.1155</v>
+      </c>
+      <c r="Z45" t="n">
+        <v>8.684200000000001</v>
       </c>
       <c r="AA45" t="inlineStr">
         <is>
@@ -6243,10 +5979,8 @@
           <t>AS16276 OVH SAS</t>
         </is>
       </c>
-      <c r="S46" t="inlineStr">
-        <is>
-          <t>60306</t>
-        </is>
+      <c r="S46" t="n">
+        <v>60306</v>
       </c>
       <c r="T46" t="inlineStr">
         <is>
@@ -6273,15 +6007,11 @@
           <t>EU</t>
         </is>
       </c>
-      <c r="Y46" t="inlineStr">
-        <is>
-          <t>50.1155</t>
-        </is>
-      </c>
-      <c r="Z46" t="inlineStr">
-        <is>
-          <t>8.6842</t>
-        </is>
+      <c r="Y46" t="n">
+        <v>50.1155</v>
+      </c>
+      <c r="Z46" t="n">
+        <v>8.684200000000001</v>
       </c>
       <c r="AA46" t="inlineStr">
         <is>
@@ -6370,10 +6100,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S47" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S47" t="n">
+        <v>34096</v>
       </c>
       <c r="T47" t="inlineStr">
         <is>
@@ -6400,15 +6128,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y47" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z47" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y47" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z47" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA47" t="inlineStr">
         <is>
@@ -6497,10 +6221,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S48" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S48" t="n">
+        <v>16250</v>
       </c>
       <c r="T48" t="inlineStr">
         <is>
@@ -6527,15 +6249,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y48" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z48" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y48" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z48" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA48" t="inlineStr">
         <is>
@@ -6624,10 +6342,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S49" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S49" t="n">
+        <v>34096</v>
       </c>
       <c r="T49" t="inlineStr">
         <is>
@@ -6654,15 +6370,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y49" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z49" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y49" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z49" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA49" t="inlineStr">
         <is>
@@ -6751,10 +6463,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S50" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S50" t="n">
+        <v>34096</v>
       </c>
       <c r="T50" t="inlineStr">
         <is>
@@ -6781,15 +6491,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y50" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z50" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y50" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z50" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA50" t="inlineStr">
         <is>
@@ -6878,10 +6584,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S51" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S51" t="n">
+        <v>34096</v>
       </c>
       <c r="T51" t="inlineStr">
         <is>
@@ -6908,15 +6612,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y51" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z51" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y51" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z51" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA51" t="inlineStr">
         <is>
@@ -7005,10 +6705,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S52" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S52" t="n">
+        <v>34096</v>
       </c>
       <c r="T52" t="inlineStr">
         <is>
@@ -7035,15 +6733,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y52" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z52" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y52" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z52" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA52" t="inlineStr">
         <is>
@@ -7132,10 +6826,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S53" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S53" t="n">
+        <v>34096</v>
       </c>
       <c r="T53" t="inlineStr">
         <is>
@@ -7162,15 +6854,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y53" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z53" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y53" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z53" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA53" t="inlineStr">
         <is>
@@ -7259,10 +6947,8 @@
           <t>AS16276 OVH SAS</t>
         </is>
       </c>
-      <c r="S54" t="inlineStr">
-        <is>
-          <t>60306</t>
-        </is>
+      <c r="S54" t="n">
+        <v>60306</v>
       </c>
       <c r="T54" t="inlineStr">
         <is>
@@ -7289,15 +6975,11 @@
           <t>EU</t>
         </is>
       </c>
-      <c r="Y54" t="inlineStr">
-        <is>
-          <t>50.1155</t>
-        </is>
-      </c>
-      <c r="Z54" t="inlineStr">
-        <is>
-          <t>8.6842</t>
-        </is>
+      <c r="Y54" t="n">
+        <v>50.1155</v>
+      </c>
+      <c r="Z54" t="n">
+        <v>8.684200000000001</v>
       </c>
       <c r="AA54" t="inlineStr">
         <is>
@@ -7386,10 +7068,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S55" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S55" t="n">
+        <v>16250</v>
       </c>
       <c r="T55" t="inlineStr">
         <is>
@@ -7416,15 +7096,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y55" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z55" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y55" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z55" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA55" t="inlineStr">
         <is>
@@ -7513,10 +7189,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S56" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S56" t="n">
+        <v>16250</v>
       </c>
       <c r="T56" t="inlineStr">
         <is>
@@ -7543,15 +7217,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y56" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z56" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y56" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z56" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA56" t="inlineStr">
         <is>
@@ -7640,10 +7310,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S57" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S57" t="n">
+        <v>16250</v>
       </c>
       <c r="T57" t="inlineStr">
         <is>
@@ -7670,15 +7338,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y57" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z57" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y57" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z57" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA57" t="inlineStr">
         <is>
@@ -7767,10 +7431,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S58" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S58" t="n">
+        <v>16250</v>
       </c>
       <c r="T58" t="inlineStr">
         <is>
@@ -7797,15 +7459,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y58" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z58" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y58" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z58" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA58" t="inlineStr">
         <is>
@@ -7894,10 +7552,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S59" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S59" t="n">
+        <v>34096</v>
       </c>
       <c r="T59" t="inlineStr">
         <is>
@@ -7924,15 +7580,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y59" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z59" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y59" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z59" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA59" t="inlineStr">
         <is>
@@ -8021,10 +7673,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S60" t="inlineStr">
-        <is>
-          <t>35210</t>
-        </is>
+      <c r="S60" t="n">
+        <v>35210</v>
       </c>
       <c r="T60" t="inlineStr">
         <is>
@@ -8051,15 +7701,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y60" t="inlineStr">
-        <is>
-          <t>38.4127</t>
-        </is>
-      </c>
-      <c r="Z60" t="inlineStr">
-        <is>
-          <t>27.1384</t>
-        </is>
+      <c r="Y60" t="n">
+        <v>38.4127</v>
+      </c>
+      <c r="Z60" t="n">
+        <v>27.1384</v>
       </c>
       <c r="AA60" t="inlineStr">
         <is>
@@ -8148,10 +7794,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S61" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S61" t="n">
+        <v>16250</v>
       </c>
       <c r="T61" t="inlineStr">
         <is>
@@ -8178,15 +7822,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y61" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z61" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y61" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z61" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA61" t="inlineStr">
         <is>
@@ -8275,10 +7915,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S62" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S62" t="n">
+        <v>16250</v>
       </c>
       <c r="T62" t="inlineStr">
         <is>
@@ -8305,15 +7943,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y62" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z62" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y62" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z62" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA62" t="inlineStr">
         <is>
@@ -8402,10 +8036,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S63" t="inlineStr">
-        <is>
-          <t>34096</t>
-        </is>
+      <c r="S63" t="n">
+        <v>34096</v>
       </c>
       <c r="T63" t="inlineStr">
         <is>
@@ -8432,15 +8064,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y63" t="inlineStr">
-        <is>
-          <t>41.0138</t>
-        </is>
-      </c>
-      <c r="Z63" t="inlineStr">
-        <is>
-          <t>28.9497</t>
-        </is>
+      <c r="Y63" t="n">
+        <v>41.0138</v>
+      </c>
+      <c r="Z63" t="n">
+        <v>28.9497</v>
       </c>
       <c r="AA63" t="inlineStr">
         <is>
@@ -8529,10 +8157,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S64" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S64" t="n">
+        <v>16250</v>
       </c>
       <c r="T64" t="inlineStr">
         <is>
@@ -8559,15 +8185,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y64" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z64" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y64" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z64" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA64" t="inlineStr">
         <is>
@@ -8656,10 +8278,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S65" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S65" t="n">
+        <v>16250</v>
       </c>
       <c r="T65" t="inlineStr">
         <is>
@@ -8686,15 +8306,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y65" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z65" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y65" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z65" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA65" t="inlineStr">
         <is>
@@ -8783,10 +8399,8 @@
           <t>AS42846 GNET Internet Telekomunikasyon A.S.</t>
         </is>
       </c>
-      <c r="S66" t="inlineStr">
-        <is>
-          <t>16250</t>
-        </is>
+      <c r="S66" t="n">
+        <v>16250</v>
       </c>
       <c r="T66" t="inlineStr">
         <is>
@@ -8813,15 +8427,11 @@
           <t>AS</t>
         </is>
       </c>
-      <c r="Y66" t="inlineStr">
-        <is>
-          <t>40.1956</t>
-        </is>
-      </c>
-      <c r="Z66" t="inlineStr">
-        <is>
-          <t>29.0601</t>
-        </is>
+      <c r="Y66" t="n">
+        <v>40.1956</v>
+      </c>
+      <c r="Z66" t="n">
+        <v>29.0601</v>
       </c>
       <c r="AA66" t="inlineStr">
         <is>
@@ -8910,10 +8520,8 @@
           <t>AS16276 OVH SAS</t>
         </is>
       </c>
-      <c r="S67" t="inlineStr">
-        <is>
-          <t>60306</t>
-        </is>
+      <c r="S67" t="n">
+        <v>60306</v>
       </c>
       <c r="T67" t="inlineStr">
         <is>
@@ -8940,15 +8548,11 @@
           <t>EU</t>
         </is>
       </c>
-      <c r="Y67" t="inlineStr">
-        <is>
-          <t>50.1155</t>
-        </is>
-      </c>
-      <c r="Z67" t="inlineStr">
-        <is>
-          <t>8.6842</t>
-        </is>
+      <c r="Y67" t="n">
+        <v>50.1155</v>
+      </c>
+      <c r="Z67" t="n">
+        <v>8.684200000000001</v>
       </c>
       <c r="AA67" t="inlineStr">
         <is>
@@ -9037,10 +8641,8 @@
           <t>AS16276 OVH SAS</t>
         </is>
       </c>
-      <c r="S68" t="inlineStr">
-        <is>
-          <t>60306</t>
-        </is>
+      <c r="S68" t="n">
+        <v>60306</v>
       </c>
       <c r="T68" t="inlineStr">
         <is>
@@ -9067,15 +8669,11 @@
           <t>EU</t>
         </is>
       </c>
-      <c r="Y68" t="inlineStr">
-        <is>
-          <t>50.1155</t>
-        </is>
-      </c>
-      <c r="Z68" t="inlineStr">
-        <is>
-          <t>8.6842</t>
-        </is>
+      <c r="Y68" t="n">
+        <v>50.1155</v>
+      </c>
+      <c r="Z68" t="n">
+        <v>8.684200000000001</v>
       </c>
       <c r="AA68" t="inlineStr">
         <is>

</xml_diff>